<commit_message>
working on exporting method
</commit_message>
<xml_diff>
--- a/cellstyle.xlsx
+++ b/cellstyle.xlsx
@@ -151,7 +151,7 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s" s="1">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
@@ -161,10 +161,10 @@
         <v>54.0</v>
       </c>
       <c r="G2" t="n">
-        <v>125.0</v>
+        <v>126.0</v>
       </c>
       <c r="H2" t="n">
-        <v>142.0</v>
+        <v>141.0</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Refactored the method writeFile
</commit_message>
<xml_diff>
--- a/cellstyle.xlsx
+++ b/cellstyle.xlsx
@@ -12,45 +12,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>user_name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>followsCount</t>
+  </si>
+  <si>
+    <t>followedByCount</t>
+  </si>
+  <si>
+    <t>profilePicUrl</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>biography</t>
+  </si>
+  <si>
+    <t>fullName</t>
+  </si>
+  <si>
+    <t>mediaCount</t>
+  </si>
+  <si>
+    <t>isPrivate</t>
+  </si>
+  <si>
+    <t>externalUrl</t>
+  </si>
+  <si>
+    <t>isVerified</t>
   </si>
   <si>
     <t>alexander_tor</t>
   </si>
   <si>
-    <t>full_name</t>
+    <t>126</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>https://scontent-frt3-2.cdninstagram.com/t51.2885-19/s150x150/12547223_1224254634256001_1551784283_a.jpg</t>
+  </si>
+  <si>
+    <t>1617365128</t>
+  </si>
+  <si>
+    <t>Too young to be settled down</t>
   </si>
   <si>
     <t>Alexander</t>
   </si>
   <si>
-    <t>bio</t>
-  </si>
-  <si>
-    <t>Too young to be settled down</t>
-  </si>
-  <si>
-    <t>profile_pic_url</t>
-  </si>
-  <si>
-    <t>https://scontent-frx5-1.cdninstagram.com/t51.2885-19/s150x150/12547223_1224254634256001_1551784283_a.jpg</t>
-  </si>
-  <si>
-    <t>media_count</t>
-  </si>
-  <si>
-    <t>following_count</t>
-  </si>
-  <si>
-    <t>followed_by</t>
-  </si>
-  <si>
-    <t>is_private</t>
+    <t>54</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>empty</t>
   </si>
 </sst>
 </file>
@@ -106,10 +130,13 @@
     <col min="2" max="2" width="15.625" customWidth="true"/>
     <col min="3" max="3" width="15.625" customWidth="true"/>
     <col min="4" max="4" width="15.625" customWidth="true"/>
-    <col min="5" max="5" width="31.25" customWidth="true"/>
+    <col min="5" max="5" width="15.625" customWidth="true"/>
     <col min="6" max="6" width="15.625" customWidth="true"/>
     <col min="7" max="7" width="15.625" customWidth="true"/>
     <col min="8" max="8" width="15.625" customWidth="true"/>
+    <col min="9" max="9" width="15.625" customWidth="true"/>
+    <col min="10" max="10" width="15.625" customWidth="true"/>
+    <col min="11" max="11" width="15.625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -120,54 +147,66 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1.617365128E9</v>
+      <c r="A2" t="s">
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="n">
-        <v>54.0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>126.0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>141.0</v>
-      </c>
-      <c r="I2" t="b">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>